<commit_message>
add visus.ipynb and update rqs tables
</commit_message>
<xml_diff>
--- a/granularidade_grossa/results/compact_result_table_civil_without_duplicates.xlsx
+++ b/granularidade_grossa/results/compact_result_table_civil_without_duplicates.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -711,36 +711,32 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>one_shot</t>
-        </is>
-      </c>
+      <c r="A9" s="2" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
           <t>mistral-nemo_12b</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.846</v>
+        <v>0.819</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0.776</v>
+        <v>0.923</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.868</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.738</v>
+        <v>0.798</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0.708</v>
+        <v>0.701</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>697</v>
+        <v>1009</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>1105</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10">
@@ -751,25 +747,25 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.819</v>
+        <v>0.805</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.9360000000000001</v>
+        <v>0.953</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.874</v>
+        <v>0.872</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.806</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>0.704</v>
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>0.681</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>1022</v>
+        <v>1143</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>315</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11">
@@ -780,29 +776,33 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.834</v>
+        <v>0.825</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.923</v>
+        <v>0.946</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.876</v>
+        <v>0.881</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.8120000000000001</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.726</v>
+        <v>0.716</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>911</v>
+        <v>994</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>380</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n"/>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>one_shot</t>
+        </is>
+      </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
           <t>deepseek-r1_8b</t>
@@ -918,36 +918,32 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>few_shot</t>
-        </is>
-      </c>
+      <c r="A16" s="2" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
           <t>llama3.1_8b</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0.788</v>
+        <v>0.799</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.948</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0.861</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0.779</v>
+        <v>0.783</v>
       </c>
       <c r="G16" s="3" t="n">
-        <v>0.648</v>
+        <v>0.666</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>1262</v>
+        <v>1163</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>257</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17">
@@ -958,25 +954,25 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0.786</v>
+        <v>0.849</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.929</v>
+        <v>0.735</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0.852</v>
+        <v>0.788</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0.767</v>
+        <v>0.715</v>
       </c>
       <c r="G17" s="3" t="n">
-        <v>0.642</v>
+        <v>0.7</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>1247</v>
+        <v>649</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>353</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="18">
@@ -987,25 +983,25 @@
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.8110000000000001</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.927</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0.865</v>
+        <v>0.866</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0.792</v>
+        <v>0.793</v>
       </c>
       <c r="G18" s="3" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>1067</v>
+        <v>1100</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>361</v>
+        <v>326</v>
       </c>
     </row>
     <row r="19">
@@ -1016,25 +1012,25 @@
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.836</v>
+        <v>0.846</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0.806</v>
+        <v>0.776</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.821</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0.747</v>
+        <v>0.738</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>0.701</v>
+        <v>0.708</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>779</v>
+        <v>697</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>960</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="20">
@@ -1045,25 +1041,25 @@
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.824</v>
+        <v>0.819</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>0.928</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.873</v>
+        <v>0.874</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0.805</v>
+        <v>0.806</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>0.71</v>
+        <v>0.704</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>983</v>
+        <v>1022</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>356</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21">
@@ -1077,26 +1073,30 @@
         <v>0.834</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0.929</v>
+        <v>0.923</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0.879</v>
+        <v>0.876</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0.8149999999999999</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>0.727</v>
+        <v>0.726</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>352</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n"/>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>few_shot</t>
+        </is>
+      </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
           <t>deepseek-r1_8b</t>
@@ -1125,36 +1125,32 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>auto_cot</t>
-        </is>
-      </c>
+      <c r="A23" s="2" t="n"/>
       <c r="B23" s="1" t="inlineStr">
         <is>
           <t>deepseek-r1_14b</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.771</v>
+        <v>0.736</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>0.981</v>
+        <v>0.996</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.863</v>
+        <v>0.846</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0.777</v>
+        <v>0.74</v>
       </c>
       <c r="G23" s="3" t="n">
-        <v>0.618</v>
+        <v>0.542</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>1440</v>
+        <v>1764</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>95</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -1165,25 +1161,25 @@
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.836</v>
+        <v>0.84</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>0.654</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>0.734</v>
+        <v>0.592</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>0.694</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>0.659</v>
+        <v>0.625</v>
       </c>
       <c r="G24" s="3" t="n">
-        <v>0.663</v>
+        <v>0.652</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>635</v>
+        <v>558</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>1710</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="25">
@@ -1194,25 +1190,25 @@
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.834</v>
+        <v>0.823</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>0.888</v>
+        <v>0.915</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.86</v>
+        <v>0.867</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>0.792</v>
+        <v>0.798</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>0.718</v>
+        <v>0.706</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>875</v>
+        <v>971</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>552</v>
+        <v>420</v>
       </c>
     </row>
     <row r="26">
@@ -1223,25 +1219,25 @@
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.801</v>
+        <v>0.788</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>0.9429999999999999</v>
+        <v>0.948</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.866</v>
+        <v>0.861</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>0.791</v>
+        <v>0.779</v>
       </c>
       <c r="G26" s="3" t="n">
-        <v>0.672</v>
+        <v>0.648</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>1158</v>
+        <v>1262</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>282</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27">
@@ -1252,25 +1248,25 @@
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.861</v>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>0.556</v>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>0.676</v>
-      </c>
-      <c r="F27" s="3" t="n">
-        <v>0.616</v>
+        <v>0.786</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0.929</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>0.767</v>
       </c>
       <c r="G27" s="3" t="n">
-        <v>0.663</v>
+        <v>0.642</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>445</v>
+        <v>1247</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>2194</v>
+        <v>353</v>
       </c>
     </row>
     <row r="28">
@@ -1281,25 +1277,25 @@
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.766</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0.978</v>
+        <v>0.927</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>0.859</v>
+        <v>0.865</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>0.77</v>
+        <v>0.792</v>
       </c>
       <c r="G28" s="3" t="n">
-        <v>0.608</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>1476</v>
+        <v>1067</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>107</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29">
@@ -1310,58 +1306,54 @@
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.836</v>
       </c>
       <c r="D29" s="2" t="n">
+        <v>0.806</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0.821</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>0.747</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>0.701</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>779</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n"/>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>phi4_14b</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>0.824</v>
+      </c>
+      <c r="D30" s="2" t="n">
         <v>0.928</v>
       </c>
-      <c r="E29" s="2" t="n">
-        <v>0.865</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <v>0.792</v>
-      </c>
-      <c r="G29" s="3" t="n">
-        <v>0.6860000000000001</v>
-      </c>
-      <c r="H29" s="2" t="n">
-        <v>1076</v>
-      </c>
-      <c r="I29" s="2" t="n">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>role_based</t>
-        </is>
-      </c>
-      <c r="B30" s="1" t="inlineStr">
-        <is>
-          <t>phi4_14b</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="n">
-        <v>0.832</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>0.917</v>
-      </c>
       <c r="E30" s="2" t="n">
-        <v>0.872</v>
+        <v>0.873</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>0.722</v>
+        <v>0.71</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>916</v>
+        <v>983</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>411</v>
+        <v>356</v>
       </c>
     </row>
     <row r="31">
@@ -1372,54 +1364,58 @@
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>0.854</v>
+        <v>0.834</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>0.92</v>
+        <v>0.929</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.886</v>
+        <v>0.879</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>0.829</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>0.759</v>
+        <v>0.727</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>778</v>
+        <v>917</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>397</v>
+        <v>352</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="n"/>
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>auto_cot</t>
+        </is>
+      </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
           <t>deepseek-r1_8b</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0.741</v>
+        <v>0.772</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0.995</v>
+        <v>0.963</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0.85</v>
+        <v>0.857</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>0.747</v>
+        <v>0.769</v>
       </c>
       <c r="G32" s="3" t="n">
-        <v>0.554</v>
+        <v>0.619</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>1716</v>
+        <v>1403</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>24</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33">
@@ -1430,25 +1426,25 @@
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>0.819</v>
+        <v>0.771</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>0.948</v>
+        <v>0.981</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>0.879</v>
+        <v>0.863</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>0.8120000000000001</v>
-      </c>
-      <c r="G33" s="2" t="n">
-        <v>0.706</v>
+        <v>0.777</v>
+      </c>
+      <c r="G33" s="3" t="n">
+        <v>0.618</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>1036</v>
+        <v>1440</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>256</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34">
@@ -1459,25 +1455,25 @@
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>0.821</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>0.902</v>
+        <v>0.836</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>0.654</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="F34" s="2" t="n">
-        <v>0.789</v>
-      </c>
-      <c r="G34" s="2" t="n">
-        <v>0.701</v>
+        <v>0.734</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="G34" s="3" t="n">
+        <v>0.663</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>969</v>
+        <v>635</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>484</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="35">
@@ -1488,25 +1484,25 @@
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>0.8179999999999999</v>
+        <v>0.834</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>0.93</v>
+        <v>0.888</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0.87</v>
+        <v>0.86</v>
       </c>
       <c r="F35" s="2" t="n">
-        <v>0.801</v>
+        <v>0.792</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>0.701</v>
+        <v>0.718</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>1022</v>
+        <v>875</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>348</v>
+        <v>552</v>
       </c>
     </row>
     <row r="36">
@@ -1517,58 +1513,54 @@
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>0.84</v>
+        <v>0.801</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>0.906</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>0.872</v>
+        <v>0.866</v>
       </c>
       <c r="F36" s="2" t="n">
-        <v>0.8080000000000001</v>
-      </c>
-      <c r="G36" s="2" t="n">
-        <v>0.732</v>
+        <v>0.791</v>
+      </c>
+      <c r="G36" s="3" t="n">
+        <v>0.672</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>856</v>
+        <v>1158</v>
       </c>
       <c r="I36" s="2" t="n">
-        <v>464</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>role_based_one_shot</t>
-        </is>
-      </c>
+      <c r="A37" s="2" t="n"/>
       <c r="B37" s="1" t="inlineStr">
         <is>
           <t>llama3.2_3b</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>0.89</v>
+        <v>0.861</v>
       </c>
       <c r="D37" s="3" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>0.745</v>
+        <v>0.556</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>0.676</v>
       </c>
       <c r="F37" s="3" t="n">
-        <v>0.6840000000000001</v>
-      </c>
-      <c r="G37" s="2" t="n">
-        <v>0.719</v>
+        <v>0.616</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>0.663</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>392</v>
+        <v>445</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>1779</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="38">
@@ -1579,25 +1571,25 @@
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>0.821</v>
+        <v>0.766</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>0.919</v>
+        <v>0.978</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>0.868</v>
+        <v>0.859</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>0.798</v>
-      </c>
-      <c r="G38" s="2" t="n">
-        <v>0.704</v>
+        <v>0.77</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>0.608</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>988</v>
+        <v>1476</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>399</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39">
@@ -1608,25 +1600,25 @@
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>0.863</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D39" s="2" t="n">
+        <v>0.928</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0.865</v>
+      </c>
+      <c r="F39" s="2" t="n">
         <v>0.792</v>
       </c>
-      <c r="E39" s="2" t="n">
-        <v>0.826</v>
-      </c>
-      <c r="F39" s="2" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="G39" s="2" t="n">
-        <v>0.736</v>
+      <c r="G39" s="3" t="n">
+        <v>0.6860000000000001</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>620</v>
+        <v>1076</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>1030</v>
+        <v>354</v>
       </c>
     </row>
     <row r="40">
@@ -1637,25 +1629,25 @@
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>0.829</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>0.931</v>
+        <v>0.952</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>0.877</v>
+        <v>0.873</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>0.8120000000000001</v>
-      </c>
-      <c r="G40" s="2" t="n">
-        <v>0.72</v>
+        <v>0.802</v>
+      </c>
+      <c r="G40" s="3" t="n">
+        <v>0.6850000000000001</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>947</v>
+        <v>1125</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>343</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41">
@@ -1666,600 +1658,584 @@
         </is>
       </c>
       <c r="C41" s="2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0.9340000000000001</v>
+      </c>
+      <c r="E41" s="2" t="n">
         <v>0.879</v>
       </c>
-      <c r="D41" s="2" t="n">
-        <v>0.865</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>0.872</v>
-      </c>
       <c r="F41" s="2" t="n">
-        <v>0.8179999999999999</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>0.78</v>
+        <v>0.723</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>590</v>
+        <v>944</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>665</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>zero_shot</t>
+          <t>role_based</t>
         </is>
       </c>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>gpt-4o-mini</t>
+          <t>deepseek-r1_8b</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>0.825</v>
+        <v>0.741</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>0.946</v>
+        <v>0.995</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>0.881</v>
+        <v>0.85</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>0.8159999999999999</v>
-      </c>
-      <c r="G42" s="2" t="n">
-        <v>0.716</v>
+        <v>0.747</v>
+      </c>
+      <c r="G42" s="3" t="n">
+        <v>0.554</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>994</v>
+        <v>1716</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>269</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>mistral-nemo_12b</t>
+          <t>deepseek-r1_14b</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
         <v>0.819</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>0.923</v>
+        <v>0.948</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>0.868</v>
+        <v>0.879</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>0.798</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>0.701</v>
+        <v>0.706</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>1009</v>
+        <v>1036</v>
       </c>
       <c r="I43" s="2" t="n">
-        <v>380</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>phi4_14b</t>
+          <t>gemma_7b</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>0.805</v>
+        <v>0.821</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0.953</v>
+        <v>0.902</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>0.872</v>
+        <v>0.86</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G44" s="3" t="n">
-        <v>0.681</v>
+        <v>0.789</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <v>0.701</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>1143</v>
+        <v>969</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>234</v>
+        <v>484</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>one_shot</t>
-        </is>
-      </c>
+      <c r="A45" s="2" t="n"/>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>llama3.1_8b</t>
+          <t>gemma2_9b</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>0.799</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>0.9330000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>0.861</v>
+        <v>0.87</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>0.783</v>
-      </c>
-      <c r="G45" s="3" t="n">
-        <v>0.666</v>
+        <v>0.801</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>0.701</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>1163</v>
+        <v>1022</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>330</v>
+        <v>348</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n"/>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>llama3.2_3b</t>
+          <t>llama3.1_8b</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>0.849</v>
+        <v>0.84</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>0.735</v>
+        <v>0.906</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>0.788</v>
+        <v>0.872</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>0.715</v>
-      </c>
-      <c r="G46" s="3" t="n">
-        <v>0.7</v>
+        <v>0.8080000000000001</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <v>0.732</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>649</v>
+        <v>856</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>1308</v>
+        <v>464</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n"/>
       <c r="B47" s="1" t="inlineStr">
         <is>
+          <t>llama3.2_3b</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>0.781</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>0.8169999999999999</v>
+      </c>
+      <c r="F47" s="2" t="n">
+        <v>0.749</v>
+      </c>
+      <c r="G47" s="2" t="n">
+        <v>0.724</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>645</v>
+      </c>
+      <c r="I47" s="2" t="n">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n"/>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
           <t>mistral_7b</t>
         </is>
       </c>
-      <c r="C47" s="2" t="n">
-        <v>0.8080000000000001</v>
-      </c>
-      <c r="D47" s="2" t="n">
-        <v>0.9340000000000001</v>
-      </c>
-      <c r="E47" s="2" t="n">
-        <v>0.866</v>
-      </c>
-      <c r="F47" s="2" t="n">
-        <v>0.793</v>
-      </c>
-      <c r="G47" s="3" t="n">
-        <v>0.6830000000000001</v>
-      </c>
-      <c r="H47" s="2" t="n">
-        <v>1100</v>
-      </c>
-      <c r="I47" s="2" t="n">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>few_shot</t>
-        </is>
-      </c>
-      <c r="B48" s="1" t="inlineStr">
-        <is>
-          <t>deepseek-r1_14b</t>
-        </is>
-      </c>
       <c r="C48" s="2" t="n">
-        <v>0.736</v>
+        <v>0.777</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>0.996</v>
+        <v>0.974</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>0.846</v>
+        <v>0.864</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="G48" s="3" t="n">
-        <v>0.542</v>
+        <v>0.629</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>1764</v>
+        <v>1384</v>
       </c>
       <c r="I48" s="2" t="n">
-        <v>22</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n"/>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>gemma2_9b</t>
+          <t>mistral-nemo_12b</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>0.823</v>
+        <v>0.859</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>0.915</v>
+        <v>0.838</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>0.867</v>
+        <v>0.849</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>0.798</v>
+        <v>0.785</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>0.706</v>
+        <v>0.744</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>971</v>
+        <v>678</v>
       </c>
       <c r="I49" s="2" t="n">
-        <v>420</v>
+        <v>801</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n"/>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>gemma_7b</t>
+          <t>phi4_14b</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="D50" s="3" t="n">
-        <v>0.592</v>
-      </c>
-      <c r="E50" s="3" t="n">
-        <v>0.694</v>
-      </c>
-      <c r="F50" s="3" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="G50" s="3" t="n">
-        <v>0.652</v>
+        <v>0.832</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>0.917</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>0.872</v>
+      </c>
+      <c r="F50" s="2" t="n">
+        <v>0.8070000000000001</v>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>0.722</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>558</v>
+        <v>916</v>
       </c>
       <c r="I50" s="2" t="n">
-        <v>2019</v>
+        <v>411</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>auto_cot</t>
-        </is>
-      </c>
+      <c r="A51" s="2" t="n"/>
       <c r="B51" s="1" t="inlineStr">
         <is>
+          <t>gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>0.886</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <v>0.829</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>0.759</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>778</v>
+      </c>
+      <c r="I51" s="2" t="n">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>role_based_few_shot</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
           <t>deepseek-r1_8b</t>
         </is>
       </c>
-      <c r="C51" s="2" t="n">
-        <v>0.772</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <v>0.963</v>
-      </c>
-      <c r="E51" s="2" t="n">
-        <v>0.857</v>
-      </c>
-      <c r="F51" s="2" t="n">
-        <v>0.769</v>
-      </c>
-      <c r="G51" s="3" t="n">
-        <v>0.619</v>
-      </c>
-      <c r="H51" s="2" t="n">
-        <v>1403</v>
-      </c>
-      <c r="I51" s="2" t="n">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="2" t="n"/>
-      <c r="B52" s="1" t="inlineStr">
-        <is>
-          <t>gpt-4o-mini</t>
-        </is>
-      </c>
       <c r="C52" s="2" t="n">
-        <v>0.83</v>
+        <v>0.778</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>0.9340000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>0.879</v>
+        <v>0.843</v>
       </c>
       <c r="F52" s="2" t="n">
-        <v>0.8159999999999999</v>
-      </c>
-      <c r="G52" s="2" t="n">
-        <v>0.723</v>
+        <v>0.754</v>
+      </c>
+      <c r="G52" s="3" t="n">
+        <v>0.624</v>
       </c>
       <c r="H52" s="2" t="n">
-        <v>944</v>
+        <v>1298</v>
       </c>
       <c r="I52" s="2" t="n">
-        <v>324</v>
+        <v>397</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n"/>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>phi4_14b</t>
+          <t>deepseek-r1_14b</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.741</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>0.952</v>
+        <v>0.992</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>0.873</v>
+        <v>0.848</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>0.802</v>
+        <v>0.745</v>
       </c>
       <c r="G53" s="3" t="n">
-        <v>0.6850000000000001</v>
+        <v>0.552</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>1125</v>
+        <v>1715</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>239</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>role_based</t>
-        </is>
-      </c>
+      <c r="A54" s="2" t="n"/>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>llama3.2_3b</t>
+          <t>gemma_7b</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
-        <v>0.857</v>
+        <v>0.837</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>0.781</v>
+        <v>0.788</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>0.8169999999999999</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>0.749</v>
-      </c>
-      <c r="G54" s="2" t="n">
-        <v>0.724</v>
+        <v>0.737</v>
+      </c>
+      <c r="G54" s="3" t="n">
+        <v>0.698</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>645</v>
+        <v>759</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>1081</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n"/>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>mistral-nemo_12b</t>
+          <t>gemma2_9b</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
-        <v>0.859</v>
+        <v>0.846</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>0.838</v>
+        <v>0.89</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>0.849</v>
+        <v>0.868</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>0.785</v>
+        <v>0.805</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>0.744</v>
+        <v>0.739</v>
       </c>
       <c r="H55" s="2" t="n">
-        <v>678</v>
+        <v>799</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>801</v>
+        <v>543</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n"/>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>mistral_7b</t>
+          <t>llama3.1_8b</t>
         </is>
       </c>
       <c r="C56" s="2" t="n">
-        <v>0.777</v>
+        <v>0.834</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>0.974</v>
+        <v>0.871</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>0.864</v>
+        <v>0.852</v>
       </c>
       <c r="F56" s="2" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="G56" s="3" t="n">
-        <v>0.629</v>
+        <v>0.782</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>0.713</v>
       </c>
       <c r="H56" s="2" t="n">
-        <v>1384</v>
+        <v>859</v>
       </c>
       <c r="I56" s="2" t="n">
-        <v>127</v>
+        <v>638</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>role_based_few_shot</t>
-        </is>
-      </c>
+      <c r="A57" s="2" t="n"/>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>deepseek-r1_14b</t>
+          <t>llama3.2_3b</t>
         </is>
       </c>
       <c r="C57" s="2" t="n">
-        <v>0.741</v>
+        <v>0.849</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>0.992</v>
+        <v>0.841</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>0.848</v>
+        <v>0.845</v>
       </c>
       <c r="F57" s="2" t="n">
-        <v>0.745</v>
-      </c>
-      <c r="G57" s="3" t="n">
-        <v>0.552</v>
+        <v>0.778</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>0.729</v>
       </c>
       <c r="H57" s="2" t="n">
-        <v>1715</v>
+        <v>742</v>
       </c>
       <c r="I57" s="2" t="n">
-        <v>42</v>
+        <v>784</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n"/>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>deepseek-r1_8b</t>
+          <t>mistral_7b</t>
         </is>
       </c>
       <c r="C58" s="2" t="n">
-        <v>0.778</v>
+        <v>0.82</v>
       </c>
       <c r="D58" s="2" t="n">
         <v>0.92</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>0.843</v>
+        <v>0.867</v>
       </c>
       <c r="F58" s="2" t="n">
-        <v>0.754</v>
-      </c>
-      <c r="G58" s="3" t="n">
-        <v>0.624</v>
+        <v>0.797</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>0.702</v>
       </c>
       <c r="H58" s="2" t="n">
-        <v>1298</v>
+        <v>998</v>
       </c>
       <c r="I58" s="2" t="n">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n"/>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>gemma2_9b</t>
+          <t>mistral-nemo_12b</t>
         </is>
       </c>
       <c r="C59" s="2" t="n">
-        <v>0.846</v>
+        <v>0.839</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>0.89</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>0.868</v>
+        <v>0.828</v>
       </c>
       <c r="F59" s="2" t="n">
-        <v>0.805</v>
+        <v>0.756</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>0.739</v>
+        <v>0.708</v>
       </c>
       <c r="H59" s="2" t="n">
-        <v>799</v>
+        <v>774</v>
       </c>
       <c r="I59" s="2" t="n">
-        <v>543</v>
+        <v>906</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n"/>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>gemma_7b</t>
+          <t>phi4_14b</t>
         </is>
       </c>
       <c r="C60" s="2" t="n">
-        <v>0.837</v>
+        <v>0.828</v>
       </c>
       <c r="D60" s="2" t="n">
-        <v>0.788</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>0.8120000000000001</v>
+        <v>0.878</v>
       </c>
       <c r="F60" s="2" t="n">
-        <v>0.737</v>
-      </c>
-      <c r="G60" s="3" t="n">
-        <v>0.698</v>
+        <v>0.8139999999999999</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>0.719</v>
       </c>
       <c r="H60" s="2" t="n">
-        <v>759</v>
+        <v>962</v>
       </c>
       <c r="I60" s="2" t="n">
-        <v>1046</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61">
@@ -2292,297 +2268,297 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="n"/>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>role_based_one_shot</t>
+        </is>
+      </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>llama3.1_8b</t>
+          <t>deepseek-r1_8b</t>
         </is>
       </c>
       <c r="C62" s="2" t="n">
-        <v>0.834</v>
+        <v>0.785</v>
       </c>
       <c r="D62" s="2" t="n">
-        <v>0.871</v>
+        <v>0.946</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>0.852</v>
+        <v>0.858</v>
       </c>
       <c r="F62" s="2" t="n">
-        <v>0.782</v>
-      </c>
-      <c r="G62" s="2" t="n">
-        <v>0.713</v>
+        <v>0.775</v>
+      </c>
+      <c r="G62" s="3" t="n">
+        <v>0.641</v>
       </c>
       <c r="H62" s="2" t="n">
-        <v>859</v>
+        <v>1283</v>
       </c>
       <c r="I62" s="2" t="n">
-        <v>638</v>
+        <v>266</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n"/>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>llama3.2_3b</t>
+          <t>deepseek-r1_14b</t>
         </is>
       </c>
       <c r="C63" s="2" t="n">
-        <v>0.849</v>
+        <v>0.747</v>
       </c>
       <c r="D63" s="2" t="n">
-        <v>0.841</v>
+        <v>0.99</v>
       </c>
       <c r="E63" s="2" t="n">
-        <v>0.845</v>
+        <v>0.851</v>
       </c>
       <c r="F63" s="2" t="n">
-        <v>0.778</v>
-      </c>
-      <c r="G63" s="2" t="n">
-        <v>0.729</v>
+        <v>0.752</v>
+      </c>
+      <c r="G63" s="3" t="n">
+        <v>0.5659999999999999</v>
       </c>
       <c r="H63" s="2" t="n">
-        <v>742</v>
+        <v>1659</v>
       </c>
       <c r="I63" s="2" t="n">
-        <v>784</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n"/>
       <c r="B64" s="1" t="inlineStr">
         <is>
-          <t>mistral-nemo_12b</t>
+          <t>gemma_7b</t>
         </is>
       </c>
       <c r="C64" s="2" t="n">
-        <v>0.839</v>
-      </c>
-      <c r="D64" s="2" t="n">
-        <v>0.8169999999999999</v>
+        <v>0.884</v>
+      </c>
+      <c r="D64" s="3" t="n">
+        <v>0.603</v>
       </c>
       <c r="E64" s="2" t="n">
-        <v>0.828</v>
-      </c>
-      <c r="F64" s="2" t="n">
-        <v>0.756</v>
-      </c>
-      <c r="G64" s="2" t="n">
-        <v>0.708</v>
+        <v>0.717</v>
+      </c>
+      <c r="F64" s="3" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="G64" s="3" t="n">
+        <v>0.7</v>
       </c>
       <c r="H64" s="2" t="n">
-        <v>774</v>
+        <v>393</v>
       </c>
       <c r="I64" s="2" t="n">
-        <v>906</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n"/>
       <c r="B65" s="1" t="inlineStr">
         <is>
-          <t>mistral_7b</t>
+          <t>gemma2_9b</t>
         </is>
       </c>
       <c r="C65" s="2" t="n">
-        <v>0.82</v>
+        <v>0.852</v>
       </c>
       <c r="D65" s="2" t="n">
-        <v>0.92</v>
+        <v>0.865</v>
       </c>
       <c r="E65" s="2" t="n">
-        <v>0.867</v>
+        <v>0.858</v>
       </c>
       <c r="F65" s="2" t="n">
-        <v>0.797</v>
+        <v>0.795</v>
       </c>
       <c r="G65" s="2" t="n">
-        <v>0.702</v>
+        <v>0.74</v>
       </c>
       <c r="H65" s="2" t="n">
-        <v>998</v>
+        <v>744</v>
       </c>
       <c r="I65" s="2" t="n">
-        <v>395</v>
+        <v>667</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n"/>
       <c r="B66" s="1" t="inlineStr">
         <is>
-          <t>phi4_14b</t>
+          <t>llama3.1_8b</t>
         </is>
       </c>
       <c r="C66" s="2" t="n">
-        <v>0.828</v>
+        <v>0.859</v>
       </c>
       <c r="D66" s="2" t="n">
-        <v>0.9360000000000001</v>
+        <v>0.792</v>
       </c>
       <c r="E66" s="2" t="n">
-        <v>0.878</v>
+        <v>0.824</v>
       </c>
       <c r="F66" s="2" t="n">
-        <v>0.8139999999999999</v>
+        <v>0.757</v>
       </c>
       <c r="G66" s="2" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>644</v>
+      </c>
+      <c r="I66" s="2" t="n">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n"/>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>llama3.2_3b</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="G67" s="2" t="n">
         <v>0.719</v>
       </c>
-      <c r="H66" s="2" t="n">
-        <v>962</v>
-      </c>
-      <c r="I66" s="2" t="n">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>role_based_one_shot</t>
-        </is>
-      </c>
-      <c r="B67" s="1" t="inlineStr">
-        <is>
-          <t>deepseek-r1_14b</t>
-        </is>
-      </c>
-      <c r="C67" s="2" t="n">
-        <v>0.747</v>
-      </c>
-      <c r="D67" s="2" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="E67" s="2" t="n">
-        <v>0.851</v>
-      </c>
-      <c r="F67" s="2" t="n">
-        <v>0.752</v>
-      </c>
-      <c r="G67" s="3" t="n">
-        <v>0.5659999999999999</v>
-      </c>
       <c r="H67" s="2" t="n">
-        <v>1659</v>
+        <v>392</v>
       </c>
       <c r="I67" s="2" t="n">
-        <v>49</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n"/>
       <c r="B68" s="1" t="inlineStr">
         <is>
-          <t>deepseek-r1_8b</t>
+          <t>mistral_7b</t>
         </is>
       </c>
       <c r="C68" s="2" t="n">
-        <v>0.785</v>
+        <v>0.821</v>
       </c>
       <c r="D68" s="2" t="n">
-        <v>0.946</v>
+        <v>0.919</v>
       </c>
       <c r="E68" s="2" t="n">
-        <v>0.858</v>
+        <v>0.868</v>
       </c>
       <c r="F68" s="2" t="n">
-        <v>0.775</v>
-      </c>
-      <c r="G68" s="3" t="n">
-        <v>0.641</v>
+        <v>0.798</v>
+      </c>
+      <c r="G68" s="2" t="n">
+        <v>0.704</v>
       </c>
       <c r="H68" s="2" t="n">
-        <v>1283</v>
+        <v>988</v>
       </c>
       <c r="I68" s="2" t="n">
-        <v>266</v>
+        <v>399</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n"/>
       <c r="B69" s="1" t="inlineStr">
         <is>
-          <t>gemma2_9b</t>
+          <t>mistral-nemo_12b</t>
         </is>
       </c>
       <c r="C69" s="2" t="n">
-        <v>0.852</v>
+        <v>0.863</v>
       </c>
       <c r="D69" s="2" t="n">
-        <v>0.865</v>
+        <v>0.792</v>
       </c>
       <c r="E69" s="2" t="n">
-        <v>0.858</v>
+        <v>0.826</v>
       </c>
       <c r="F69" s="2" t="n">
-        <v>0.795</v>
+        <v>0.76</v>
       </c>
       <c r="G69" s="2" t="n">
-        <v>0.74</v>
+        <v>0.736</v>
       </c>
       <c r="H69" s="2" t="n">
-        <v>744</v>
+        <v>620</v>
       </c>
       <c r="I69" s="2" t="n">
-        <v>667</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n"/>
       <c r="B70" s="1" t="inlineStr">
         <is>
-          <t>gemma_7b</t>
+          <t>phi4_14b</t>
         </is>
       </c>
       <c r="C70" s="2" t="n">
-        <v>0.884</v>
-      </c>
-      <c r="D70" s="3" t="n">
-        <v>0.603</v>
+        <v>0.829</v>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>0.931</v>
       </c>
       <c r="E70" s="2" t="n">
-        <v>0.717</v>
-      </c>
-      <c r="F70" s="3" t="n">
-        <v>0.658</v>
-      </c>
-      <c r="G70" s="3" t="n">
-        <v>0.7</v>
+        <v>0.877</v>
+      </c>
+      <c r="F70" s="2" t="n">
+        <v>0.8120000000000001</v>
+      </c>
+      <c r="G70" s="2" t="n">
+        <v>0.72</v>
       </c>
       <c r="H70" s="2" t="n">
-        <v>393</v>
+        <v>947</v>
       </c>
       <c r="I70" s="2" t="n">
-        <v>1962</v>
+        <v>343</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n"/>
       <c r="B71" s="1" t="inlineStr">
         <is>
-          <t>llama3.1_8b</t>
+          <t>gpt-4o-mini</t>
         </is>
       </c>
       <c r="C71" s="2" t="n">
-        <v>0.859</v>
+        <v>0.879</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>0.792</v>
+        <v>0.865</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>0.824</v>
+        <v>0.872</v>
       </c>
       <c r="F71" s="2" t="n">
-        <v>0.757</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="G71" s="2" t="n">
-        <v>0.73</v>
+        <v>0.78</v>
       </c>
       <c r="H71" s="2" t="n">
-        <v>644</v>
+        <v>590</v>
       </c>
       <c r="I71" s="2" t="n">
-        <v>1028</v>
+        <v>665</v>
       </c>
     </row>
     <row r="72">
@@ -2593,203 +2569,203 @@
       </c>
       <c r="B72" s="1" t="inlineStr">
         <is>
-          <t>deepseek-r1_14b</t>
+          <t>deepseek-r1_8b</t>
         </is>
       </c>
       <c r="C72" s="2" t="n">
-        <v>0.79</v>
+        <v>0.784</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>0.97</v>
+        <v>0.968</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>0.871</v>
+        <v>0.866</v>
       </c>
       <c r="F72" s="2" t="n">
-        <v>0.793</v>
+        <v>0.785</v>
       </c>
       <c r="G72" s="3" t="n">
-        <v>0.656</v>
+        <v>0.643</v>
       </c>
       <c r="H72" s="2" t="n">
-        <v>1271</v>
+        <v>1320</v>
       </c>
       <c r="I72" s="2" t="n">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n"/>
       <c r="B73" s="1" t="inlineStr">
         <is>
-          <t>deepseek-r1_8b</t>
+          <t>deepseek-r1_14b</t>
         </is>
       </c>
       <c r="C73" s="2" t="n">
-        <v>0.784</v>
+        <v>0.79</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>0.968</v>
+        <v>0.97</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>0.866</v>
+        <v>0.871</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>0.785</v>
+        <v>0.793</v>
       </c>
       <c r="G73" s="3" t="n">
-        <v>0.643</v>
+        <v>0.656</v>
       </c>
       <c r="H73" s="2" t="n">
-        <v>1320</v>
+        <v>1271</v>
       </c>
       <c r="I73" s="2" t="n">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n"/>
       <c r="B74" s="1" t="inlineStr">
         <is>
-          <t>gemma2_9b</t>
+          <t>gemma_7b</t>
         </is>
       </c>
       <c r="C74" s="2" t="n">
-        <v>0.83</v>
+        <v>0.824</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>0.909</v>
+        <v>0.878</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>0.868</v>
+        <v>0.85</v>
       </c>
       <c r="F74" s="2" t="n">
-        <v>0.801</v>
-      </c>
-      <c r="G74" s="2" t="n">
-        <v>0.717</v>
+        <v>0.777</v>
+      </c>
+      <c r="G74" s="3" t="n">
+        <v>0.699</v>
       </c>
       <c r="H74" s="2" t="n">
-        <v>921</v>
+        <v>927</v>
       </c>
       <c r="I74" s="2" t="n">
-        <v>448</v>
+        <v>604</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n"/>
       <c r="B75" s="1" t="inlineStr">
         <is>
-          <t>gemma_7b</t>
+          <t>gemma2_9b</t>
         </is>
       </c>
       <c r="C75" s="2" t="n">
-        <v>0.824</v>
+        <v>0.83</v>
       </c>
       <c r="D75" s="2" t="n">
-        <v>0.878</v>
+        <v>0.909</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>0.85</v>
+        <v>0.868</v>
       </c>
       <c r="F75" s="2" t="n">
-        <v>0.777</v>
-      </c>
-      <c r="G75" s="3" t="n">
-        <v>0.699</v>
+        <v>0.801</v>
+      </c>
+      <c r="G75" s="2" t="n">
+        <v>0.717</v>
       </c>
       <c r="H75" s="2" t="n">
-        <v>927</v>
+        <v>921</v>
       </c>
       <c r="I75" s="2" t="n">
-        <v>604</v>
+        <v>448</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n"/>
       <c r="B76" s="1" t="inlineStr">
         <is>
-          <t>gpt-4o-mini</t>
+          <t>llama3.1_8b</t>
         </is>
       </c>
       <c r="C76" s="2" t="n">
-        <v>0.857</v>
+        <v>0.827</v>
       </c>
       <c r="D76" s="2" t="n">
-        <v>0.899</v>
+        <v>0.922</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>0.877</v>
+        <v>0.872</v>
       </c>
       <c r="F76" s="2" t="n">
-        <v>0.819</v>
+        <v>0.805</v>
       </c>
       <c r="G76" s="2" t="n">
-        <v>0.757</v>
+        <v>0.715</v>
       </c>
       <c r="H76" s="2" t="n">
-        <v>742</v>
+        <v>951</v>
       </c>
       <c r="I76" s="2" t="n">
-        <v>501</v>
+        <v>388</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n"/>
       <c r="B77" s="1" t="inlineStr">
         <is>
-          <t>llama3.1_8b</t>
+          <t>llama3.2_3b</t>
         </is>
       </c>
       <c r="C77" s="2" t="n">
-        <v>0.827</v>
+        <v>0.864</v>
       </c>
       <c r="D77" s="2" t="n">
-        <v>0.922</v>
+        <v>0.742</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>0.872</v>
+        <v>0.798</v>
       </c>
       <c r="F77" s="2" t="n">
-        <v>0.805</v>
+        <v>0.731</v>
       </c>
       <c r="G77" s="2" t="n">
-        <v>0.715</v>
+        <v>0.722</v>
       </c>
       <c r="H77" s="2" t="n">
-        <v>951</v>
+        <v>577</v>
       </c>
       <c r="I77" s="2" t="n">
-        <v>388</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n"/>
       <c r="B78" s="1" t="inlineStr">
         <is>
-          <t>llama3.2_3b</t>
+          <t>mistral_7b</t>
         </is>
       </c>
       <c r="C78" s="2" t="n">
-        <v>0.864</v>
+        <v>0.766</v>
       </c>
       <c r="D78" s="2" t="n">
-        <v>0.742</v>
+        <v>0.983</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>0.798</v>
+        <v>0.861</v>
       </c>
       <c r="F78" s="2" t="n">
-        <v>0.731</v>
-      </c>
-      <c r="G78" s="2" t="n">
-        <v>0.722</v>
+        <v>0.772</v>
+      </c>
+      <c r="G78" s="3" t="n">
+        <v>0.607</v>
       </c>
       <c r="H78" s="2" t="n">
-        <v>577</v>
+        <v>1488</v>
       </c>
       <c r="I78" s="2" t="n">
-        <v>1275</v>
+        <v>83</v>
       </c>
     </row>
     <row r="79">
@@ -2825,58 +2801,58 @@
       <c r="A80" s="2" t="n"/>
       <c r="B80" s="1" t="inlineStr">
         <is>
-          <t>mistral_7b</t>
+          <t>phi4_14b</t>
         </is>
       </c>
       <c r="C80" s="2" t="n">
-        <v>0.766</v>
+        <v>0.834</v>
       </c>
       <c r="D80" s="2" t="n">
-        <v>0.983</v>
+        <v>0.896</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>0.861</v>
+        <v>0.864</v>
       </c>
       <c r="F80" s="2" t="n">
-        <v>0.772</v>
-      </c>
-      <c r="G80" s="3" t="n">
-        <v>0.607</v>
+        <v>0.797</v>
+      </c>
+      <c r="G80" s="2" t="n">
+        <v>0.72</v>
       </c>
       <c r="H80" s="2" t="n">
-        <v>1488</v>
+        <v>881</v>
       </c>
       <c r="I80" s="2" t="n">
-        <v>83</v>
+        <v>513</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n"/>
       <c r="B81" s="1" t="inlineStr">
         <is>
-          <t>phi4_14b</t>
+          <t>gpt-4o-mini</t>
         </is>
       </c>
       <c r="C81" s="2" t="n">
-        <v>0.834</v>
+        <v>0.857</v>
       </c>
       <c r="D81" s="2" t="n">
-        <v>0.896</v>
+        <v>0.899</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>0.864</v>
+        <v>0.877</v>
       </c>
       <c r="F81" s="2" t="n">
-        <v>0.797</v>
+        <v>0.819</v>
       </c>
       <c r="G81" s="2" t="n">
-        <v>0.72</v>
+        <v>0.757</v>
       </c>
       <c r="H81" s="2" t="n">
-        <v>881</v>
+        <v>742</v>
       </c>
       <c r="I81" s="2" t="n">
-        <v>513</v>
+        <v>501</v>
       </c>
     </row>
     <row r="82">
@@ -2938,21 +2914,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A57:A66"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="A2:A8"/>
+  <mergeCells count="8">
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="A62:A71"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A52:A61"/>
+    <mergeCell ref="A42:A51"/>
     <mergeCell ref="A72:A81"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="A22:A31"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>